<commit_message>
Signed-off-by: STUDENT Jack Patterson <Jack.Patterson@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00217640\Desktop\Computer-Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC5E5CA-2D3E-4B83-84D6-0D220AF5CA1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B34FFA1-F15B-4F13-829B-2620850C066A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>z = -1</t>
   </si>
@@ -165,79 +164,19 @@
     <t>Vertices of your letter</t>
   </si>
   <si>
-    <t xml:space="preserve">0    ,   0    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2    ,   4    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3    ,   4    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2    ,   3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3    ,   3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1    ,   3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   -2    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1    ,   -2    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   -3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3    ,   -2    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3    ,   -3    ,    0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   0    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2    ,   4    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3    ,   4    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2    ,   3    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3    ,   3    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1    ,   3    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   3    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   -2    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1    ,   -2    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0    ,   -3    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3    ,   -2    ,    -0.5    ,    </t>
-  </si>
-  <si>
-    <t>-3    ,   -3    ,    -0.5</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>0    0    0    1</t>
+  </si>
+  <si>
+    <t>3.999529    0.04701208    -0.03947484    -5</t>
+  </si>
+  <si>
+    <t>-0.02960613    2.9546    0.5190982    -1</t>
+  </si>
+  <si>
+    <t>0.01175302    -0.1729149    0.9848666    2</t>
   </si>
 </sst>
 </file>
@@ -461,7 +400,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -540,9 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -576,38 +512,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -674,6 +610,494 @@
         <a:xfrm>
           <a:off x="3000375" y="371475"/>
           <a:ext cx="1143000" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2924175</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>857250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CE61B86-0071-47F7-BB94-2014C634629A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2219325" y="4705350"/>
+          <a:ext cx="2533650" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3057525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3914775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0C4318E-082A-4B18-A72F-F43FEE9F143B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2152650" y="5972175"/>
+          <a:ext cx="2733675" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A221DFA-1C9C-4122-8A4A-15D3EFBB6D69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3067050" y="10344150"/>
+          <a:ext cx="857250" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2924175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3905250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CB195E-B9B6-473D-B405-F887E685751F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2190750" y="11325225"/>
+          <a:ext cx="2562225" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2085975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1E25EF-1080-43FC-8B9A-820C5828EC66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3105150" y="15621000"/>
+          <a:ext cx="809625" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2914650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6832D4BE-B381-43F3-9836-67BBE944EDA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2190750" y="16602075"/>
+          <a:ext cx="2552700" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C2116D5-35BA-434A-B134-F8F5B9FA76F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7448550" y="16602075"/>
+          <a:ext cx="2552700" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>733425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3C9EFD-139F-4B5B-8E8A-9DD2BFA89530}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7467600" y="10334625"/>
+          <a:ext cx="2552700" cy="657225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1019,7 +1443,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1033,25 +1457,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="K2" s="28" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="K2" s="27" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1069,7 +1493,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1080,7 +1504,7 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <f>MOD(C4,100)-50</f>
         <v>-10</v>
       </c>
@@ -1092,15 +1516,15 @@
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <f>INT((C4/10000))-5</f>
         <v>16</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>1</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>1</v>
       </c>
@@ -1112,19 +1536,18 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="31">
-        <f>INT((C4/10000))-5</f>
-        <v>16</v>
-      </c>
-      <c r="D8" s="31">
+      <c r="C8" s="30">
+        <v>4</v>
+      </c>
+      <c r="D8" s="30">
         <f>MOD(INT((C4/1000)),10)-4</f>
         <v>3</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>1</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="31" t="s">
         <v>38</v>
       </c>
       <c r="L8" t="s">
@@ -1138,15 +1561,15 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <f>MOD(C4,10)-5</f>
         <v>-5</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <f>MOD(INT((C4/10)),10)-5</f>
         <v>-1</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <f>MOD(INT((C4/100)),10)-4</f>
         <v>2</v>
       </c>
@@ -1158,15 +1581,15 @@
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <f>2+C7</f>
         <v>18</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <f>3+D7</f>
         <v>4</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <f>E7+50</f>
         <v>51</v>
       </c>
@@ -1176,15 +1599,15 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="28">
         <f>D7</f>
         <v>1</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="28">
         <f>C8</f>
-        <v>16</v>
-      </c>
-      <c r="E12" s="29">
+        <v>4</v>
+      </c>
+      <c r="E12" s="28">
         <f>E8</f>
         <v>1</v>
       </c>
@@ -1194,15 +1617,15 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <f>E9</f>
         <v>2</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <f>D7</f>
         <v>1</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="28">
         <f>C7</f>
         <v>16</v>
       </c>
@@ -1233,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1256,7 +1679,7 @@
     </row>
     <row r="2" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="8"/>
@@ -1269,8 +1692,8 @@
     </row>
     <row r="3" spans="3:12" ht="316.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="34" t="s">
-        <v>65</v>
+      <c r="D3" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="11"/>
@@ -1290,7 +1713,7 @@
     </row>
     <row r="5" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="8"/>
@@ -1301,7 +1724,7 @@
     </row>
     <row r="6" spans="3:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="34"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="15"/>
@@ -1320,7 +1743,7 @@
     </row>
     <row r="8" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="17"/>
@@ -1330,9 +1753,9 @@
       <c r="K8" s="15"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="3:12" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:12" ht="312.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="34"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="17"/>
       <c r="F9" s="12"/>
       <c r="G9" s="15"/>
@@ -1351,26 +1774,26 @@
     </row>
     <row r="11" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="43"/>
+      <c r="H11" s="46"/>
       <c r="I11" s="8"/>
       <c r="K11" s="15"/>
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="3:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="34"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="46"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="16"/>
       <c r="J12" s="12"/>
       <c r="K12" s="15"/>
@@ -1389,7 +1812,7 @@
     </row>
     <row r="14" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="32" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="17"/>
@@ -1401,9 +1824,9 @@
       <c r="K14" s="15"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="3:12" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:12" ht="309" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="34"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="17"/>
       <c r="F15" s="12"/>
       <c r="G15" s="15"/>
@@ -1426,7 +1849,7 @@
     </row>
     <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18"/>
@@ -1440,7 +1863,7 @@
     </row>
     <row r="18" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="34"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="20"/>
       <c r="G18" s="15"/>
       <c r="H18" s="12"/>
@@ -1460,29 +1883,29 @@
     </row>
     <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="42" t="s">
+      <c r="F20" s="43"/>
+      <c r="G20" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="43"/>
+      <c r="H20" s="46"/>
       <c r="I20" s="17"/>
       <c r="J20" s="12"/>
       <c r="K20" s="15"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="307.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="46"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="47"/>
       <c r="I21" s="17"/>
       <c r="J21" s="12"/>
       <c r="K21" s="15"/>
@@ -1499,7 +1922,7 @@
     </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="9"/>
@@ -1508,22 +1931,22 @@
       <c r="H23" s="22"/>
       <c r="I23" s="10"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="42" t="s">
+      <c r="K23" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="43"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="34"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="6"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="7"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="46"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="47"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1535,7 +1958,7 @@
     <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="12"/>
@@ -1548,7 +1971,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="12"/>
       <c r="I27" s="15"/>
       <c r="J27" s="12"/>
@@ -1565,12 +1988,12 @@
       <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="32" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="9"/>
@@ -1583,10 +2006,10 @@
       <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="34"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="20"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -1603,42 +2026,42 @@
       <c r="L31" s="8"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="41"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="40" t="s">
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="41"/>
+      <c r="L32" s="38"/>
     </row>
     <row r="33" spans="1:12" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="39"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="39"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="40"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1649,40 +2072,35 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="34"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E38" s="26"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="39"/>
-    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
+  <mergeCells count="16">
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1693,137 +2111,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06E9F78-0195-43AB-BDBC-0F00F160EFB5}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A24"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>64</v>
-      </c>
-    </row>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Assignment 1 done, texturing done Signed-off-by: STUDENT Jack Patterson <Jack.Patterson@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00217640\Desktop\Computer-Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CF1DE2-DDA4-43E1-8767-DA7FEF5D0C54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC767A5A-6BDD-4077-9C7B-794F973726AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -512,13 +512,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -536,14 +539,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -588,6 +588,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:noFill/>
@@ -1019,6 +1030,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:noFill/>
@@ -4128,8 +4150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4252,10 +4274,10 @@
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="47"/>
       <c r="I11" s="8"/>
       <c r="K11" s="15"/>
       <c r="L11" s="12"/>
@@ -4265,8 +4287,8 @@
       <c r="D12" s="33"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="16"/>
       <c r="J12" s="12"/>
       <c r="K12" s="15"/>
@@ -4362,11 +4384,11 @@
       <c r="E20" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="37" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="38"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="17"/>
       <c r="J20" s="12"/>
       <c r="K20" s="15"/>
@@ -4376,9 +4398,9 @@
       <c r="C21" s="5"/>
       <c r="D21" s="33"/>
       <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
       <c r="I21" s="17"/>
       <c r="J21" s="12"/>
       <c r="K21" s="15"/>
@@ -4404,10 +4426,10 @@
       <c r="H23" s="22"/>
       <c r="I23" s="10"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="38"/>
+      <c r="L23" s="47"/>
     </row>
     <row r="24" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
@@ -4418,8 +4440,8 @@
       <c r="H24" s="11"/>
       <c r="I24" s="7"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="43"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -4461,10 +4483,10 @@
       <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="25"/>
       <c r="D29" s="32" t="s">
         <v>15</v>
@@ -4479,8 +4501,8 @@
       <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" ht="309.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="25"/>
       <c r="D30" s="33"/>
       <c r="E30" s="20"/>
@@ -4499,10 +4521,10 @@
       <c r="L31" s="8"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
@@ -4512,29 +4534,29 @@
       <c r="E32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="43" t="s">
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="44"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:12" ht="306.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="45"/>
-      <c r="B33" s="46"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="17"/>
       <c r="D33" s="33"/>
       <c r="E33" s="39"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="43"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -4557,22 +4579,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K32:L32"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="E32:J32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4585,8 +4607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46795688-FD8C-42B4-BA6E-54D2CF58E5DE}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>